<commit_message>
Adds graticule to paleomaps
Improves paleomap visualization by adding a graticule (latitude and longitude lines).

No pude arreglar que el mapa aparezca cortado a los costados.
</commit_message>
<xml_diff>
--- a/data/formation_data_cyathocarpus.xlsx
+++ b/data/formation_data_cyathocarpus.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3db8b9dcb961099d/2025_03_05_Manuscrito00_Cyathocarpus/MapsCyathocarpus/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\OneDrive\Paleomaps\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="8_{6AB24570-A45D-478E-A08F-921EC0093816}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8303995F-8490-4A70-A963-5DCCF64398BE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A288AC8D-13AA-4AB3-8000-CB3965E1C289}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4290" yWindow="780" windowWidth="15375" windowHeight="7785" xr2:uid="{606E2648-BD4E-40E9-82FE-89F86083D2E4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{606E2648-BD4E-40E9-82FE-89F86083D2E4}"/>
   </bookViews>
   <sheets>
     <sheet name="SpatialChronoStrat" sheetId="1" r:id="rId1"/>
@@ -161,7 +161,7 @@
     <t>C</t>
   </si>
   <si>
-    <t>Formation</t>
+    <t>formation</t>
   </si>
 </sst>
 </file>
@@ -534,7 +534,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>